<commit_message>
Lead Source Code design updates #576
</commit_message>
<xml_diff>
--- a/design/Design Specification - Capture - GH576 - CR Lead Source Codes.xlsx
+++ b/design/Design Specification - Capture - GH576 - CR Lead Source Codes.xlsx
@@ -258,7 +258,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +276,13 @@
     </font>
     <font>
       <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -302,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -362,14 +369,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -414,6 +429,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -722,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,304 +752,314 @@
     <col min="1" max="1" width="10.140625" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="80.28515625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B3" s="20" t="s">
         <v>0</v>
       </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="21" t="s">
         <v>50</v>
       </c>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="20"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="19"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="17"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="16"/>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="14"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="9" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="10" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="8" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="9" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="8" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="8" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="F7:I7"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F5:I5"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -1060,6 +1091,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA3C61B63E22AE4CB214999D07CAFF9A" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c1d488d220c474b08f9f1957c0227932">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -1173,12 +1210,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1189,6 +1220,21 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F52DAB4A-4E17-489D-BB3D-A746C267F2E2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CE8D614-0B41-44C0-BC72-75C9D02547DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1204,21 +1250,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F52DAB4A-4E17-489D-BB3D-A746C267F2E2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3548E551-9E26-45A8-91FE-FAAB4546DA96}">
   <ds:schemaRefs>

</xml_diff>